<commit_message>
add cancel button and its action listener
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/business_trip.xlsx
+++ b/src/main/webapp/WEB-INF/book/business_trip.xlsx
@@ -210,6 +210,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -217,13 +221,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>63500</xdr:colOff>
+          <xdr:colOff>76200</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>1473200</xdr:colOff>
+          <xdr:colOff>1485900</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>139700</xdr:rowOff>
         </xdr:to>
@@ -404,6 +408,73 @@
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
                 <a:t>Reject</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1003300</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>139700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="cancel" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica"/>
+                  <a:ea typeface="Helvetica"/>
+                  <a:cs typeface="Helvetica"/>
+                </a:rPr>
+                <a:t>Cancel</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -682,7 +753,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +783,7 @@
       </c>
       <c r="F3" s="3">
         <f ca="1">TODAY()</f>
-        <v>43370</v>
+        <v>43375</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="24" x14ac:dyDescent="0.2">
@@ -724,7 +795,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>43370</v>
+        <v>43375</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>3</v>
@@ -786,13 +857,13 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>1473200</xdr:colOff>
+                    <xdr:colOff>1485900</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>139700</xdr:rowOff>
                   </to>
@@ -848,6 +919,29 @@
           </mc:Choice>
           <mc:Fallback/>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId6" name="cancel">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1003300</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>139700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
     <mc:Fallback/>

</xml_diff>

<commit_message>
apply Lauren's template design
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/business_trip.xlsx
+++ b/src/main/webapp/WEB-INF/book/business_trip.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33620" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Leave" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="arrangement">Sheet1!$A$1:$A$4</definedName>
+    <definedName name="arrangment">Sheet1!$A$1:$A$4</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,45 +32,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Date:</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Period of 
-Leave</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>From</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Days in 
-Total</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>To</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Applicant</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUSINESS TRIP</t>
-  </si>
-  <si>
-    <t>Reason</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Purpose of business trip</t>
+  </si>
+  <si>
+    <t>Business Travel Request</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period </t>
+  </si>
+  <si>
+    <t>Days in Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Associated Project Number</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Need  arrangement</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Accomondation</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Employee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,30 +103,107 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF808080"/>
-      <name val="Monaco"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E474E"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF1E474E"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF1E474E"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1E474E"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,18 +212,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF1E474E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDF2F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9E7DD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -126,70 +262,174 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFB9E7DD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF1E474E"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB9E7DD"/>
+      <color rgb="FFE4EAEA"/>
+      <color rgb="FF1E474E"/>
+      <color rgb="FFEDF2F5"/>
+      <color rgb="FFF4F4EB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -220,16 +460,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>317500</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>406400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>1485900</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>1752600</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -287,23 +527,90 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>850900</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>406400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>1485900</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="approve" hidden="1">
+            <xdr:cNvPr id="1028" name="cancel" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica"/>
+                  <a:ea typeface="Helvetica"/>
+                  <a:cs typeface="Helvetica"/>
+                </a:rPr>
+                <a:t>Cancel</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>317500</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>1752600</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>508000</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="approve" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -354,23 +661,23 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1003300</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>850900</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>508000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="reject" hidden="1">
+            <xdr:cNvPr id="1034" name="reject" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
+                  <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -408,73 +715,6 @@
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
                 <a:t>Reject</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1003300</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1031" name="cancel" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1031"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
-                </a:rPr>
-                <a:t>Cancel</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -750,101 +990,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="31" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="2:13" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="2:13" ht="37" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" ht="23" x14ac:dyDescent="0.2">
+      <c r="B4" s="4"/>
+      <c r="C4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="2:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="18">
+        <f ca="1">TODAY()</f>
+        <v>43378</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="2:13" ht="23" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="J6" s="33">
         <f ca="1">TODAY()</f>
-        <v>43375</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B4" s="11" t="s">
+        <v>43378</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <f ca="1">TODAY()</f>
-        <v>43375</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="12">
-        <f ca="1">IF(NETWORKDAYS(D4,D5) &lt; 0, 0, NETWORKDAYS(D4,D5))</f>
+      <c r="L6" s="33"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="19">
+        <f ca="1">IF(NETWORKDAYS(J6,L6) &lt; 0, 0, NETWORKDAYS(J6,L6))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B5" s="11"/>
-      <c r="C5" s="7" t="s">
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="2:13" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="2:13" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+    </row>
+    <row r="11" spans="2:13" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="23"/>
+      <c r="C11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="8"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="23"/>
+    </row>
+    <row r="12" spans="2:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="23"/>
+    </row>
+    <row r="13" spans="2:13" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="23"/>
+    </row>
+    <row r="14" spans="2:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="23"/>
+      <c r="C14" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+    </row>
+    <row r="15" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="23"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+    </row>
+    <row r="16" spans="2:13" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="23"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C6:F6"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
+  <mergeCells count="11">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:H12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23">
+      <formula1>$C$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18">
+      <formula1>"$C$18,$C$19,$C$20,$C$21,$C$22,$C$23"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:E14">
+      <formula1>arrangement</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -856,16 +1311,16 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>317500</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>406400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>1485900</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>139700</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>1752600</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -875,20 +1330,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId4" name="approve">
+            <control shapeId="1028" r:id="rId4" name="cancel">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>850900</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>406400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>1485900</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>76200</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -898,20 +1353,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId5" name="reject">
+            <control shapeId="1033" r:id="rId5" name="approve">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>1003300</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>317500</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>63500</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>76200</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>1752600</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>508000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -921,20 +1376,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId6" name="cancel">
+            <control shapeId="1034" r:id="rId6" name="reject">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>1003300</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>850900</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>63500</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>139700</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>508000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -946,5 +1401,52 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet1!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F14:G14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>